<commit_message>
major revisions but it worked out
</commit_message>
<xml_diff>
--- a/raster_cells_per_sub.xlsx
+++ b/raster_cells_per_sub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savan\OneDrive - University of Virginia\StreamLit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D2EDF6-5DAB-43A9-9BF3-5E70347EB671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1852C1EA-C39D-4C6D-B25B-A0AA6EB64147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{97454CBC-327E-48EE-B8D6-214EE2D65EB7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>NAME</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>Percent_Imp_to_perv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average </t>
   </si>
 </sst>
 </file>
@@ -283,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -295,8 +292,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,11 +629,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA42"/>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -922,7 +917,7 @@
         <v>15.37732239744</v>
       </c>
       <c r="Z3" s="8">
-        <f t="shared" ref="Z3:Z40" si="13">T3/O3*100</f>
+        <f>T3/O3*100</f>
         <v>31.659951651893635</v>
       </c>
     </row>
@@ -1017,7 +1012,7 @@
         <v>10.053492313600001</v>
       </c>
       <c r="Z4" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="Z4:Z40" si="13">T4/O4*100</f>
         <v>14.26272130741612</v>
       </c>
     </row>
@@ -3676,7 +3671,7 @@
         <v>29.62918944616116</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
@@ -3771,7 +3766,7 @@
         <v>38.374092873023194</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -3866,7 +3861,7 @@
         <v>32.410846953937593</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -3961,7 +3956,7 @@
         <v>32.011942278984904</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -4056,7 +4051,7 @@
         <v>27.475057559478124</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -4151,7 +4146,7 @@
         <v>42.414752957550448</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -4246,7 +4241,7 @@
         <v>29.56315611242804</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -4341,7 +4336,7 @@
         <v>22.821640811916335</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -4436,19 +4431,9 @@
         <v>25.863146670588666</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="U41" s="10"/>
-      <c r="Z41" s="9">
-        <f>AVERAGE(Z2:Z40)</f>
-        <v>31.332951704119512</v>
-      </c>
-      <c r="AA41" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="U42" s="6"/>
-      <c r="W42" s="5"/>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="U41" s="6"/>
+      <c r="W41" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:X1" xr:uid="{E6ED4D1B-D86F-42A9-8609-27B9E315963A}">

</xml_diff>